<commit_message>
completed JavaScript course with CodeCademy
</commit_message>
<xml_diff>
--- a/certificates.xlsx
+++ b/certificates.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rusla\Documents\Certificates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruslan Bergenov\RD\Data-Science-Certificates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013918C5-03D4-48B9-840A-797838AA93A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED76DCC-188D-43AA-B8BE-7FB7107D21AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20910" yWindow="1515" windowWidth="8385" windowHeight="12180" xr2:uid="{1A997AAC-BB89-4DC0-926B-F38AF9B432F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{1A997AAC-BB89-4DC0-926B-F38AF9B432F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="61">
   <si>
     <t>Analyzing and Visualizing Data with Power BI</t>
   </si>
@@ -193,6 +193,36 @@
   </si>
   <si>
     <t>GTM</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>Learn JavaScript Course</t>
+  </si>
+  <si>
+    <t>Platform</t>
+  </si>
+  <si>
+    <t>CodeCademy</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>DataCamp</t>
+  </si>
+  <si>
+    <t>Coursera</t>
+  </si>
+  <si>
+    <t>EdX</t>
+  </si>
+  <si>
+    <t>Learn Python 2 Course</t>
+  </si>
+  <si>
+    <t>Python</t>
   </si>
 </sst>
 </file>
@@ -200,7 +230,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -231,11 +261,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -254,13 +290,14 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruslan Bergenov" refreshedDate="44068.575841203703" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="38" xr:uid="{7F2EC5B6-FB95-440B-B5B1-43A81DEAA866}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ruslan Bergenov" refreshedDate="44190.630423495371" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="39" xr:uid="{7F2EC5B6-FB95-440B-B5B1-43A81DEAA866}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:C1048576" sheet="Sheet1"/>
+    <worksheetSource ref="A1:D1048576" sheet="Sheet1"/>
   </cacheSource>
-  <cacheFields count="3">
+  <cacheFields count="4">
     <cacheField name="Group" numFmtId="0">
-      <sharedItems containsBlank="1" count="8">
+      <sharedItems containsBlank="1" count="9">
+        <s v="JavaScript"/>
         <s v="GTM"/>
         <s v="Image Processing Pre-Req and Courses"/>
         <s v="GCP"/>
@@ -274,8 +311,11 @@
     <cacheField name="Course" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
-    <cacheField name="Date completed" numFmtId="165">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2017-09-13T00:00:00" maxDate="2020-08-19T00:00:00"/>
+    <cacheField name="Platform" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Date completed" numFmtId="164">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2017-09-13T00:00:00" maxDate="2020-12-25T00:00:00"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -287,194 +327,238 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="38">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="39">
   <r>
     <x v="0"/>
+    <s v="Learn JavaScript Course"/>
+    <s v="CodeCademy"/>
+    <d v="2020-12-24T00:00:00"/>
+  </r>
+  <r>
+    <x v="1"/>
     <s v="Google Tag Manager Fundamentals"/>
+    <s v="Google"/>
     <d v="2020-08-18T00:00:00"/>
   </r>
   <r>
-    <x v="1"/>
+    <x v="2"/>
     <s v="Supervised Learning with scikit-learn"/>
+    <s v="DataCamp"/>
     <d v="2020-08-04T00:00:00"/>
   </r>
   <r>
-    <x v="1"/>
+    <x v="2"/>
     <s v="Biomedical Image Analysis in Python"/>
+    <s v="DataCamp"/>
     <d v="2020-07-03T00:00:00"/>
   </r>
   <r>
-    <x v="1"/>
+    <x v="2"/>
     <s v="Image Processing in Python"/>
+    <s v="DataCamp"/>
     <d v="2020-06-22T00:00:00"/>
   </r>
   <r>
-    <x v="1"/>
+    <x v="2"/>
     <s v="Python Data Science Toolbox (Part 2)"/>
+    <s v="DataCamp"/>
     <d v="2020-06-14T00:00:00"/>
   </r>
   <r>
-    <x v="2"/>
+    <x v="3"/>
     <s v="4 Applying Machine Learning to your Data with GCP"/>
+    <s v="Coursera"/>
     <d v="2020-05-02T00:00:00"/>
   </r>
   <r>
-    <x v="2"/>
+    <x v="3"/>
     <s v="3 Achieving Advanced Insights with BigQuery"/>
+    <s v="Coursera"/>
     <d v="2020-04-22T00:00:00"/>
   </r>
   <r>
-    <x v="2"/>
+    <x v="3"/>
     <s v="2 Creating New BigQuery Datasets and Visualizing Insights"/>
+    <s v="Coursera"/>
     <d v="2020-04-12T00:00:00"/>
   </r>
   <r>
-    <x v="2"/>
+    <x v="3"/>
     <s v="1 Exploring and Preparing your Data with BigQuery"/>
+    <s v="Coursera"/>
     <d v="2020-03-23T00:00:00"/>
   </r>
   <r>
-    <x v="2"/>
+    <x v="3"/>
     <s v="From Data to Insights with Google Cloud Platform"/>
+    <s v="Coursera"/>
     <d v="2020-02-05T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Data Analyst with Python Track"/>
+    <s v="DataCamp"/>
     <d v="2019-08-06T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Statistical Thinking in Python (Part 2)"/>
+    <s v="DataCamp"/>
     <d v="2019-08-06T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Statistical Thinking in Python (Part 1)"/>
+    <s v="DataCamp"/>
     <d v="2019-07-26T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Introduction to Relational Databases in SQL"/>
+    <s v="DataCamp"/>
     <d v="2019-07-21T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Joining Data in SQL"/>
+    <s v="DataCamp"/>
     <d v="2019-07-16T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Intro to SQL for Data Science"/>
+    <s v="DataCamp"/>
     <d v="2019-07-04T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Introduction to Data Science in Python"/>
+    <s v="DataCamp"/>
     <d v="2019-06-29T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Introduction to Data Visualization with Python"/>
+    <s v="DataCamp"/>
     <d v="2019-06-28T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Analyzing Police Activity with pandas"/>
+    <s v="DataCamp"/>
     <d v="2019-06-20T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Merging DataFrames with pandas"/>
+    <s v="DataCamp"/>
     <d v="2019-06-15T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Manipulating DataFrames with pandas"/>
+    <s v="DataCamp"/>
     <d v="2019-05-31T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="pandas Foundations"/>
+    <s v="DataCamp"/>
     <d v="2019-05-10T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Cleaning Data in Python"/>
+    <s v="DataCamp"/>
     <d v="2019-04-25T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Importing Data in Python (Part 2)"/>
+    <s v="DataCamp"/>
     <d v="2019-04-05T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Importing Data in Python (Part 1)"/>
+    <s v="DataCamp"/>
     <d v="2019-03-27T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Python Data Science Toolbox (Part 1)"/>
+    <s v="DataCamp"/>
     <d v="2019-03-24T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Intermediate Python for Data Science"/>
+    <s v="DataCamp"/>
     <d v="2019-03-19T00:00:00"/>
   </r>
   <r>
-    <x v="4"/>
+    <x v="5"/>
     <s v="Introduction to Time Series Analysis"/>
+    <s v="DataCamp"/>
     <d v="2019-03-06T00:00:00"/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <s v="Introduction to Python"/>
+    <s v="DataCamp"/>
     <d v="2018-09-12T00:00:00"/>
   </r>
   <r>
-    <x v="4"/>
+    <x v="5"/>
     <s v="Intermediate R"/>
+    <s v="DataCamp"/>
     <d v="2018-07-22T00:00:00"/>
   </r>
   <r>
-    <x v="4"/>
+    <x v="5"/>
     <s v="Inference for Linear Regression"/>
+    <s v="DataCamp"/>
     <d v="2018-06-26T00:00:00"/>
   </r>
   <r>
-    <x v="4"/>
+    <x v="5"/>
     <s v="Exploratory Data Analysis"/>
+    <s v="DataCamp"/>
     <d v="2018-06-07T00:00:00"/>
   </r>
   <r>
-    <x v="4"/>
+    <x v="5"/>
     <s v="Foundations of Inference"/>
+    <s v="DataCamp"/>
     <d v="2018-06-07T00:00:00"/>
   </r>
   <r>
-    <x v="4"/>
+    <x v="5"/>
     <s v="Multiple and Logistic Regression"/>
+    <s v="DataCamp"/>
     <d v="2018-05-26T00:00:00"/>
   </r>
   <r>
-    <x v="4"/>
+    <x v="5"/>
     <s v="Correlation and Regression"/>
+    <s v="DataCamp"/>
     <d v="2018-04-29T00:00:00"/>
   </r>
   <r>
-    <x v="5"/>
+    <x v="6"/>
     <s v="SAS Programming 1: Essentials"/>
+    <s v="SAS"/>
     <d v="2018-04-18T00:00:00"/>
   </r>
   <r>
-    <x v="6"/>
+    <x v="7"/>
     <s v="Analyzing and Visualizing Data with Power BI"/>
+    <s v="EdX"/>
     <d v="2017-09-13T00:00:00"/>
   </r>
   <r>
-    <x v="7"/>
+    <x v="8"/>
+    <m/>
     <m/>
     <m/>
   </r>
@@ -482,29 +566,31 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5590EAD5-8AF3-4E7A-8773-B42689393C7A}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5590EAD5-8AF3-4E7A-8773-B42689393C7A}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A3:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="9">
+      <items count="10">
+        <item x="4"/>
         <item x="3"/>
         <item x="2"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item x="7"/>
         <item x="1"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="7"/>
-        <item x="6"/>
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
     <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="9">
+  <rowItems count="10">
     <i>
       <x/>
     </i>
@@ -528,6 +614,9 @@
     </i>
     <i>
       <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
     </i>
     <i t="grand">
       <x/>
@@ -848,452 +937,595 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6984627A-BD75-499D-905F-7B92AB309F64}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="A1:E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>50</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="3">
         <v>44061</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="3">
-        <v>44047</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="3">
-        <v>44015</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="3">
+        <v>44047</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="3">
-        <v>44004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="3">
+        <v>44015</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
       <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="3">
+        <v>44004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="3">
         <v>43996</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3">
-        <v>43953</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="3">
-        <v>43943</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="3">
+        <v>43953</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3">
-        <v>43933</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="3">
+        <v>43943</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3">
-        <v>43913</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="3">
+        <v>43933</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
       <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="3">
+        <v>43913</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="3">
         <v>43866</v>
       </c>
-      <c r="D11">
+      <c r="E12">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="3">
         <v>43683</v>
       </c>
-      <c r="D12">
+      <c r="E13">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="3">
         <v>43683</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="3">
         <v>43672</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="3">
         <v>43667</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="3">
         <v>43662</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="3">
         <v>43650</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="3">
         <v>43645</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="3">
         <v>43644</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="3">
         <v>43636</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="3">
         <v>43631</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="3">
         <v>43616</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="3">
         <v>43595</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="3">
         <v>43580</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="3">
         <v>43560</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="3">
         <v>43551</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="3">
         <v>43548</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="3">
         <v>43543</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>35</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="3">
         <v>43530</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="3">
         <v>43355</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="3">
-        <v>43303</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="3">
-        <v>43277</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="3">
+        <v>43303</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="3">
-        <v>43258</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="3">
+        <v>43277</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="3">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="3">
         <v>43258</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" s="3">
-        <v>43246</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="3">
+        <v>43258</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" s="3">
+        <v>43246</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="3">
         <v>43219</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>33</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C38" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" s="3">
         <v>43208</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="3">
+        <v>43108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>45</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B40" t="s">
         <v>0</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" s="3">
         <v>42991</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D38">
-    <sortCondition descending="1" ref="C4:C38"/>
-    <sortCondition ref="B4:B38"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E40">
+    <sortCondition descending="1" ref="D2:D40"/>
+    <sortCondition ref="B2:B40"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1302,10 +1534,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E85EC9-3AC5-4C74-BC0C-EC4F9F021474}">
-  <dimension ref="A3:B12"/>
+  <dimension ref="A3:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" activeCellId="2" sqref="B8 B6 B4"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,10 +1618,18 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="2">
-        <v>37</v>
+      <c r="B13" s="2">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>